<commit_message>
Importing assets now working
</commit_message>
<xml_diff>
--- a/test-assets.xlsx
+++ b/test-assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\Projects\twospace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7468136-BABB-4148-80A0-91552E28B75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06393663-E951-46BF-AA78-8F0008975D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B8341F0-AC8B-4AFD-9CDA-0F59B1A2CC13}"/>
   </bookViews>
@@ -25,44 +25,44 @@
     <t>description</t>
   </si>
   <si>
-    <t>SN16345</t>
-  </si>
-  <si>
     <t>HP EliteBook 840 G7</t>
   </si>
   <si>
-    <t>SN16346</t>
-  </si>
-  <si>
     <t>Dell OptiPlex 7080</t>
   </si>
   <si>
-    <t>SN16347</t>
-  </si>
-  <si>
     <t>iPad Air 4</t>
   </si>
   <si>
-    <t>SN16348</t>
-  </si>
-  <si>
     <t>iPhone 13</t>
   </si>
   <si>
-    <t>SN16349</t>
-  </si>
-  <si>
     <t>Dell UltraSharp U2720Q</t>
   </si>
   <si>
-    <t>serial_number</t>
+    <t>serialNumber</t>
+  </si>
+  <si>
+    <t>SN18123</t>
+  </si>
+  <si>
+    <t>SN18124</t>
+  </si>
+  <si>
+    <t>SN18125</t>
+  </si>
+  <si>
+    <t>SN18126</t>
+  </si>
+  <si>
+    <t>SN18127</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +193,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -919,7 +925,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +936,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -938,45 +944,46 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>